<commit_message>
inv add closer to finish
</commit_message>
<xml_diff>
--- a/node ex library/express-locallibrary-tutorial/manage.xlsx
+++ b/node ex library/express-locallibrary-tutorial/manage.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED6DF98-E5D4-4D68-9A73-F04A9FD26B59}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95A343B-FD85-479A-AF6C-64B72F3478F9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22440" yWindow="-4275" windowWidth="20055" windowHeight="15810" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22830" yWindow="-4275" windowWidth="22095" windowHeight="15810" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tasks" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>tasks view</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>change main layout view</t>
+  </si>
+  <si>
+    <t>ADD RETURN</t>
+  </si>
+  <si>
+    <t>in invoice layout</t>
   </si>
 </sst>
 </file>
@@ -133,7 +139,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,12 +164,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -178,13 +178,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -615,10 +614,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB373A26-C6AF-47E1-9CFA-0D75B84347F7}">
-  <dimension ref="B3:E15"/>
+  <dimension ref="B3:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,7 +680,7 @@
       <c r="C14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -689,11 +688,19 @@
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
static site at entry
</commit_message>
<xml_diff>
--- a/node ex library/express-locallibrary-tutorial/manage.xlsx
+++ b/node ex library/express-locallibrary-tutorial/manage.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95A343B-FD85-479A-AF6C-64B72F3478F9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7092FD70-5577-41C7-8BD0-A3D2CFC4F927}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22830" yWindow="-4275" windowWidth="22095" windowHeight="15810" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3255" yWindow="480" windowWidth="16755" windowHeight="10155" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tasks" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>tasks view</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>in invoice layout</t>
+  </si>
+  <si>
+    <t>CREATE TOTALLY NEW MAIN MENU</t>
   </si>
 </sst>
 </file>
@@ -614,15 +617,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB373A26-C6AF-47E1-9CFA-0D75B84347F7}">
-  <dimension ref="B3:E17"/>
+  <dimension ref="B3:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
@@ -703,6 +706,11 @@
         <v>30</v>
       </c>
     </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
starting with ptpiree conv (model and controller)
</commit_message>
<xml_diff>
--- a/node ex library/express-locallibrary-tutorial/manage.xlsx
+++ b/node ex library/express-locallibrary-tutorial/manage.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D6C318-625F-4F5B-939A-68AA2D12AFED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAB6EE9-045F-4EDE-9441-E688B7B8CA6C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21270" yWindow="-4350" windowWidth="13440" windowHeight="15885" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22440" yWindow="-4215" windowWidth="21885" windowHeight="15750" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tasks" sheetId="2" r:id="rId1"/>
     <sheet name="tests" sheetId="1" r:id="rId2"/>
     <sheet name="log and auth" sheetId="3" r:id="rId3"/>
     <sheet name="invoices" sheetId="4" r:id="rId4"/>
+    <sheet name="ptpiree conv" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
   <si>
     <t>tasks view</t>
   </si>
@@ -155,6 +156,66 @@
   </si>
   <si>
     <t>with link to pay method with id</t>
+  </si>
+  <si>
+    <t>models:</t>
+  </si>
+  <si>
+    <t>ptpiree_content</t>
+  </si>
+  <si>
+    <t>head</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>values</t>
+  </si>
+  <si>
+    <t>obj to file</t>
+  </si>
+  <si>
+    <t>methods:</t>
+  </si>
+  <si>
+    <t>How does it work</t>
+  </si>
+  <si>
+    <t>1. import csv file with full content (1line = 1output file)</t>
+  </si>
+  <si>
+    <t>full auto or high managable</t>
+  </si>
+  <si>
+    <t>2. convert every line into obj</t>
+  </si>
+  <si>
+    <t>3. add every obj to array</t>
+  </si>
+  <si>
+    <t>4. conv obj to file</t>
+  </si>
+  <si>
+    <t>5. add to arch or other array</t>
+  </si>
+  <si>
+    <t>6. download</t>
+  </si>
+  <si>
+    <t>send via post/get/other</t>
+  </si>
+  <si>
+    <t>OR easy way line by line</t>
+  </si>
+  <si>
+    <t>1. conv string to array</t>
+  </si>
+  <si>
+    <t>2. array pos to file line</t>
   </si>
 </sst>
 </file>
@@ -655,7 +716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB373A26-C6AF-47E1-9CFA-0D75B84347F7}">
   <dimension ref="A3:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
@@ -821,4 +882,108 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E4267D-138F-4F7F-BFE1-BDA31C215947}">
+  <dimension ref="D1:O12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>